<commit_message>
updating location lat and long name
</commit_message>
<xml_diff>
--- a/data-raw/metadata/2022_update/Location_attributes_2022.xlsx
+++ b/data-raw/metadata/2022_update/Location_attributes_2022.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10709"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10719"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maddeerubenson/Documents/git/CVPIA/edi.996.1/data-raw/metadata/2022_update/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68E59982-97D6-D04C-8410-AE7C6FC06825}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A811328F-4B4C-4D4F-A7CB-664A8E9154F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16020" xr2:uid="{EA408BAE-6FB1-4BF4-81C8-CFC6B96C724F}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15880" xr2:uid="{EA408BAE-6FB1-4BF4-81C8-CFC6B96C724F}"/>
   </bookViews>
   <sheets>
     <sheet name="attribute" sheetId="1" r:id="rId1"/>
@@ -94,9 +94,6 @@
     <t>attribute_name</t>
   </si>
   <si>
-    <t>Lat, lon (UTM)</t>
-  </si>
-  <si>
     <t>Latitude and Longitude at sample site</t>
   </si>
   <si>
@@ -112,10 +109,13 @@
     <t xml:space="preserve">monitoring or experimental </t>
   </si>
   <si>
-    <t>sample site habitat type, borad</t>
-  </si>
-  <si>
     <t>sample site habitat type, refined</t>
+  </si>
+  <si>
+    <t>sample site habitat type, broad</t>
+  </si>
+  <si>
+    <t>Lat Long UTM</t>
   </si>
 </sst>
 </file>
@@ -473,7 +473,7 @@
   <dimension ref="A1:N6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -546,10 +546,10 @@
     </row>
     <row r="3" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3" t="s">
         <v>22</v>
-      </c>
-      <c r="B3" t="s">
-        <v>23</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>16</v>
@@ -563,7 +563,7 @@
     </row>
     <row r="4" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B4" t="s">
         <v>28</v>
@@ -580,10 +580,10 @@
     </row>
     <row r="5" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>16</v>
@@ -597,10 +597,10 @@
     </row>
     <row r="6" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B6" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>16</v>
@@ -613,15 +613,21 @@
       </c>
     </row>
   </sheetData>
-  <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C6" xr:uid="{BA3C5E33-98F7-47D7-93C4-1300CC932B38}">
+  <dataValidations count="5">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C1:C6" xr:uid="{BA3C5E33-98F7-47D7-93C4-1300CC932B38}">
       <formula1>"string,boolean,decimal,float,double,duration,dateTime,time,date,gYearMonth,gYear,gMonthDay,gDay,gMonth"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D6" xr:uid="{5696B8DF-1E1E-4425-85B8-84459E8CCD16}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1:D6" xr:uid="{5696B8DF-1E1E-4425-85B8-84459E8CCD16}">
       <formula1>"nominal,ordinal,interval,ratio,dateTime"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F6" xr:uid="{45C39947-F29E-441D-8724-D5844F949A6B}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F1:F6" xr:uid="{45C39947-F29E-441D-8724-D5844F949A6B}">
       <formula1>"text,enumerated,dateTime,numeric"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G1" xr:uid="{28611BBD-6DE9-744C-9B6D-93E314C81749}">
+      <formula1>"ratio,interval"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I1" xr:uid="{E3C052FB-7282-384A-9F5F-FA10E40E7704}">
+      <formula1>"natural,whole,interger,real"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>